<commit_message>
Updated the tennis model to include player's injury process generator
Updated the tennis model to include player's injury process generator
</commit_message>
<xml_diff>
--- a/Final Project/TennisModel/Wimbledon_Model_Results.xlsx
+++ b/Final Project/TennisModel/Wimbledon_Model_Results.xlsx
@@ -494,7 +494,7 @@
         <v>6</v>
       </c>
       <c r="F3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" t="n">
         <v>6</v>
@@ -507,24 +507,24 @@
     </row>
     <row r="4">
       <c r="B4" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Roger Federer</t>
+          <t>Milos Raonic</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -540,10 +540,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>6</v>
@@ -556,21 +556,21 @@
     </row>
     <row r="6">
       <c r="B6" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Reilly Opelka</t>
+          <t>Lucas Pouille</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -586,33 +586,30 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>6</v>
       </c>
       <c r="F7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H7" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Daniil Medvedev</t>
+          <t>Matteo Berrettini</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Steve Johnson</t>
+          <t>Matteo Berrettini</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -622,13 +619,10 @@
         <v>4</v>
       </c>
       <c r="F8" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G8" t="n">
         <v>6</v>
-      </c>
-      <c r="H8" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -644,43 +638,39 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" t="n">
         <v>4</v>
       </c>
-      <c r="F9" t="n">
-        <v>7</v>
-      </c>
-      <c r="G9" t="n">
-        <v>6</v>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>David Goffin</t>
+          <t>Rafael Nadal</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Lucas Pouille</t>
+          <t>Rafael Nadal</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
         <v>6</v>
       </c>
       <c r="F10" t="n">
-        <v>6</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -696,46 +686,46 @@
         </is>
       </c>
       <c r="D11" t="n">
+        <v>6</v>
+      </c>
+      <c r="E11" t="n">
+        <v>7</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" t="n">
         <v>5</v>
       </c>
-      <c r="E11" t="n">
-        <v>6</v>
-      </c>
-      <c r="F11" t="n">
-        <v>6</v>
-      </c>
-      <c r="G11" t="n">
-        <v>3</v>
-      </c>
       <c r="H11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Kevin Anderson</t>
+          <t>Ugo Humbert</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="n">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Kevin Anderson</t>
+          <t>Ugo Humbert</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G12" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H12" t="n">
         <v>6</v>
@@ -754,49 +744,49 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G13" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H13" t="n">
         <v>6</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Fabio Fognini</t>
+          <t>Sam Querrey</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Ugo Humbert</t>
+          <t>Sam Querrey</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G14" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H14" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
@@ -812,49 +802,43 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15" t="n">
         <v>6</v>
       </c>
       <c r="F15" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G15" t="n">
-        <v>6</v>
-      </c>
-      <c r="H15" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Felix Auger Aliassime</t>
+          <t>Tennys Sandgren</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Sam Querrey</t>
+          <t>Tennys Sandgren</t>
         </is>
       </c>
       <c r="D16" t="n">
         <v>6</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F16" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G16" t="n">
-        <v>2</v>
-      </c>
-      <c r="H16" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
@@ -870,16 +854,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>6</v>
-      </c>
-      <c r="E17" t="n">
-        <v>6</v>
-      </c>
-      <c r="F17" t="n">
-        <v>6</v>
-      </c>
-      <c r="G17" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -889,24 +864,17 @@
     </row>
     <row r="18">
       <c r="B18" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Milos Raonic</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>7</v>
-      </c>
-      <c r="E18" t="n">
-        <v>3</v>
-      </c>
-      <c r="F18" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" t="n">
-        <v>4</v>
+          <t>Roberto Bautista Agut</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -922,49 +890,37 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
-        <v>2</v>
-      </c>
-      <c r="G19" t="n">
-        <v>6</v>
-      </c>
-      <c r="H19" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Kei Nishikori</t>
+          <t>Roger Federer</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Kei Nishikori</t>
+          <t>Roger Federer</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F20" t="n">
         <v>6</v>
-      </c>
-      <c r="G20" t="n">
-        <v>2</v>
-      </c>
-      <c r="H20" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="21">
@@ -980,43 +936,37 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
-        <v>6</v>
-      </c>
-      <c r="G21" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Hubert Hurkacz</t>
+          <t>Kei Nishikori</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Mikhail Kukushkin</t>
+          <t>Kei Nishikori</t>
         </is>
       </c>
       <c r="D22" t="n">
         <v>6</v>
       </c>
       <c r="E22" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
@@ -1032,13 +982,19 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E23" t="n">
         <v>7</v>
       </c>
       <c r="F23" t="n">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="G23" t="n">
+        <v>7</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1048,21 +1004,29 @@
     </row>
     <row r="24">
       <c r="B24" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Thomas Fabbiano</t>
+          <t>Steve Johnson</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E24" t="n">
         <v>6</v>
       </c>
       <c r="F24" t="n">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="G24" t="n">
+        <v>6</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1078,49 +1042,49 @@
         </is>
       </c>
       <c r="D25" t="n">
+        <v>6</v>
+      </c>
+      <c r="E25" t="n">
+        <v>6</v>
+      </c>
+      <c r="F25" t="n">
+        <v>6</v>
+      </c>
+      <c r="G25" t="n">
         <v>1</v>
       </c>
-      <c r="E25" t="n">
-        <v>6</v>
-      </c>
-      <c r="F25" t="n">
-        <v>6</v>
-      </c>
-      <c r="G25" t="n">
-        <v>5</v>
-      </c>
       <c r="H25" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Tennys Sandgren</t>
+          <t>Jiri Vesely</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Tennys Sandgren</t>
+          <t>Novak Djokovic</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G26" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H26" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1139,10 +1103,10 @@
         <v>3</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G27" t="n">
         <v>6</v>
@@ -1152,30 +1116,30 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Novak Djokovic</t>
+          <t>Mikhail Kukushkin</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Novak Djokovic</t>
+          <t>Mikhail Kukushkin</t>
         </is>
       </c>
       <c r="D28" t="n">
         <v>6</v>
       </c>
       <c r="E28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H28" t="n">
         <v>6</v>
@@ -1194,49 +1158,37 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
-        <v>6</v>
-      </c>
-      <c r="G29" t="n">
-        <v>6</v>
-      </c>
-      <c r="H29" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Joao Sousa</t>
+          <t>Kevin Anderson</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Roberto Bautista Agut</t>
+          <t>Kevin Anderson</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
-        <v>3</v>
-      </c>
-      <c r="G30" t="n">
-        <v>7</v>
-      </c>
-      <c r="H30" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
@@ -1252,43 +1204,39 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
-        <v>7</v>
-      </c>
-      <c r="G31" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Rafael Nadal</t>
+          <t>John Millman</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Rafael Nadal</t>
+          <t>Thomas Fabbiano</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E32" t="n">
         <v>6</v>
       </c>
-      <c r="F32" t="n">
-        <v>5</v>
-      </c>
-      <c r="G32" t="n">
-        <v>7</v>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -1304,13 +1252,19 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E33" t="n">
         <v>6</v>
       </c>
       <c r="F33" t="n">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" t="n">
+        <v>6</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
@@ -1320,21 +1274,27 @@
     </row>
     <row r="34">
       <c r="B34" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Matteo Berrettini</t>
+          <t>Reilly Opelka</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E34" t="n">
         <v>4</v>
       </c>
       <c r="F34" t="n">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="G34" t="n">
+        <v>6</v>
+      </c>
+      <c r="H34" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -1404,43 +1364,49 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G38" t="n">
         <v>7</v>
       </c>
+      <c r="H38" t="n">
+        <v>1</v>
+      </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Benoit Paire</t>
+          <t>Roger Federer</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Kei Nishikori</t>
+          <t>Roger Federer</t>
         </is>
       </c>
       <c r="D39" t="n">
         <v>6</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G39" t="n">
         <v>5</v>
+      </c>
+      <c r="H39" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="40">
@@ -1456,37 +1422,43 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="n">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="G40" t="n">
+        <v>4</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Daniel Evans</t>
+          <t>Kei Nishikori</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Hubert Hurkacz</t>
+          <t>Kei Nishikori</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="G41" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="42">
@@ -1494,21 +1466,27 @@
         <v>3</v>
       </c>
       <c r="B42" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Daniil Medvedev</t>
+          <t>Matteo Berrettini</t>
         </is>
       </c>
       <c r="D42" t="n">
         <v>6</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="G42" t="n">
+        <v>4</v>
+      </c>
+      <c r="H42" t="n">
+        <v>4</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
@@ -1526,12 +1504,18 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E43" t="n">
         <v>6</v>
       </c>
       <c r="F43" t="n">
+        <v>3</v>
+      </c>
+      <c r="G43" t="n">
+        <v>6</v>
+      </c>
+      <c r="H43" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1540,51 +1524,45 @@
         <v>4</v>
       </c>
       <c r="B44" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>David Goffin</t>
+          <t>Rafael Nadal</t>
         </is>
       </c>
       <c r="D44" t="n">
         <v>6</v>
       </c>
       <c r="E44" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F44" t="n">
-        <v>2</v>
-      </c>
-      <c r="G44" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Tennys Sandgren</t>
+          <t>Rafael Nadal</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Tennys Sandgren</t>
+          <t>Jiri Vesely</t>
         </is>
       </c>
       <c r="D45" t="n">
         <v>3</v>
       </c>
       <c r="E45" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F45" t="n">
-        <v>6</v>
-      </c>
-      <c r="G45" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
@@ -1592,51 +1570,51 @@
         <v>5</v>
       </c>
       <c r="B46" t="n">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Kevin Anderson</t>
+          <t>Ugo Humbert</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E46" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F46" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G46" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Novak Djokovic</t>
+          <t>Ugo Humbert</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Novak Djokovic</t>
+          <t>Mikhail Kukushkin</t>
         </is>
       </c>
       <c r="D47" t="n">
         <v>6</v>
       </c>
       <c r="E47" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F47" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G47" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
@@ -1644,51 +1622,35 @@
         <v>6</v>
       </c>
       <c r="B48" t="n">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Fabio Fognini</t>
+          <t>Sam Querrey</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>6</v>
-      </c>
-      <c r="E48" t="n">
-        <v>6</v>
-      </c>
-      <c r="F48" t="n">
         <v>5</v>
       </c>
-      <c r="G48" t="n">
-        <v>6</v>
-      </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Fabio Fognini</t>
+          <t>Sam Querrey</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Joao Sousa</t>
-        </is>
-      </c>
-      <c r="D49" t="n">
-        <v>2</v>
-      </c>
-      <c r="E49" t="n">
-        <v>4</v>
-      </c>
-      <c r="F49" t="n">
-        <v>7</v>
-      </c>
-      <c r="G49" t="n">
-        <v>4</v>
+          <t>Kevin Anderson</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -1696,45 +1658,51 @@
         <v>7</v>
       </c>
       <c r="B50" t="n">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Felix Auger Aliassime</t>
+          <t>Tennys Sandgren</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E50" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F50" t="n">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="G50" t="n">
+        <v>6</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Rafael Nadal</t>
+          <t>Tennys Sandgren</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Rafael Nadal</t>
+          <t>John Millman</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="G51" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="52">
@@ -1750,16 +1718,13 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F52" t="n">
-        <v>6</v>
-      </c>
-      <c r="G52" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
@@ -1777,16 +1742,13 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E53" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F53" t="n">
-        <v>0</v>
-      </c>
-      <c r="G53" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55">
@@ -1848,18 +1810,18 @@
         <v>1</v>
       </c>
       <c r="B57" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Benoit Paire</t>
+          <t>Roger Federer</t>
         </is>
       </c>
       <c r="D57" t="n">
         <v>6</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
         <v>6</v>
@@ -1869,27 +1831,27 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>Benoit Paire</t>
+          <t>Roger Federer</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="n">
+        <v>17</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Kei Nishikori</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>3</v>
+      </c>
+      <c r="E58" t="n">
+        <v>6</v>
+      </c>
+      <c r="F58" t="n">
         <v>2</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Daniel Evans</t>
-        </is>
-      </c>
-      <c r="D58" t="n">
-        <v>4</v>
-      </c>
-      <c r="E58" t="n">
-        <v>6</v>
-      </c>
-      <c r="F58" t="n">
-        <v>3</v>
       </c>
       <c r="G58" t="n">
         <v>4</v>
@@ -1908,49 +1870,43 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E59" t="n">
         <v>6</v>
       </c>
       <c r="F59" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G59" t="n">
-        <v>6</v>
-      </c>
-      <c r="H59" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>Tennys Sandgren</t>
+          <t>Rafael Nadal</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Tennys Sandgren</t>
+          <t>Rafael Nadal</t>
         </is>
       </c>
       <c r="D60" t="n">
         <v>6</v>
       </c>
       <c r="E60" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F60" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G60" t="n">
-        <v>4</v>
-      </c>
-      <c r="H60" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61">
@@ -1958,57 +1914,41 @@
         <v>3</v>
       </c>
       <c r="B61" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Novak Djokovic</t>
+          <t>Ugo Humbert</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E61" t="n">
-        <v>6</v>
-      </c>
-      <c r="F61" t="n">
-        <v>3</v>
-      </c>
-      <c r="G61" t="n">
-        <v>4</v>
-      </c>
-      <c r="H61" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>Novak Djokovic</t>
+          <t>Ugo Humbert</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="n">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Fabio Fognini</t>
+          <t>Sam Querrey</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>6</v>
-      </c>
-      <c r="E62" t="n">
-        <v>4</v>
-      </c>
-      <c r="F62" t="n">
-        <v>6</v>
-      </c>
-      <c r="G62" t="n">
-        <v>6</v>
-      </c>
-      <c r="H62" t="n">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
     <row r="63">
@@ -2016,31 +1956,22 @@
         <v>4</v>
       </c>
       <c r="B63" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Rafael Nadal</t>
+          <t>Tennys Sandgren</t>
         </is>
       </c>
       <c r="D63" t="n">
         <v>2</v>
       </c>
       <c r="E63" t="n">
-        <v>4</v>
-      </c>
-      <c r="F63" t="n">
-        <v>6</v>
-      </c>
-      <c r="G63" t="n">
-        <v>6</v>
-      </c>
-      <c r="H63" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>Rafael Nadal</t>
+          <t>Tennys Sandgren</t>
         </is>
       </c>
     </row>
@@ -2056,17 +1987,10 @@
       <c r="D64" t="n">
         <v>6</v>
       </c>
-      <c r="E64" t="n">
-        <v>6</v>
-      </c>
-      <c r="F64" t="n">
-        <v>1</v>
-      </c>
-      <c r="G64" t="n">
-        <v>3</v>
-      </c>
-      <c r="H64" t="n">
-        <v>0</v>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
     <row r="66">
@@ -2128,50 +2052,56 @@
         <v>1</v>
       </c>
       <c r="B68" t="n">
+        <v>27</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Roger Federer</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>6</v>
+      </c>
+      <c r="E68" t="n">
+        <v>3</v>
+      </c>
+      <c r="F68" t="n">
+        <v>3</v>
+      </c>
+      <c r="G68" t="n">
+        <v>6</v>
+      </c>
+      <c r="H68" t="n">
         <v>1</v>
       </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Benoit Paire</t>
-        </is>
-      </c>
-      <c r="D68" t="n">
-        <v>1</v>
-      </c>
-      <c r="E68" t="n">
-        <v>5</v>
-      </c>
-      <c r="F68" t="n">
-        <v>6</v>
-      </c>
-      <c r="G68" t="n">
-        <v>3</v>
-      </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>Tennys Sandgren</t>
+          <t>Rafael Nadal</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Tennys Sandgren</t>
+          <t>Rafael Nadal</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G69" t="n">
+        <v>2</v>
+      </c>
+      <c r="H69" t="n">
         <v>6</v>
       </c>
     </row>
@@ -2180,44 +2110,50 @@
         <v>2</v>
       </c>
       <c r="B70" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Novak Djokovic</t>
+          <t>Ugo Humbert</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E70" t="n">
+        <v>2</v>
+      </c>
+      <c r="F70" t="n">
         <v>1</v>
       </c>
-      <c r="F70" t="n">
+      <c r="G70" t="n">
         <v>6</v>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>Rafael Nadal</t>
+          <t>Tennys Sandgren</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Rafael Nadal</t>
+          <t>Tennys Sandgren</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E71" t="n">
         <v>6</v>
       </c>
       <c r="F71" t="n">
+        <v>6</v>
+      </c>
+      <c r="G71" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2280,51 +2216,57 @@
         <v>1</v>
       </c>
       <c r="B75" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Tennys Sandgren</t>
+          <t>Rafael Nadal</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G75" t="n">
+        <v>2</v>
+      </c>
+      <c r="H75" t="n">
         <v>6</v>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>Tennys Sandgren</t>
+          <t>Rafael Nadal</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Rafael Nadal</t>
+          <t>Tennys Sandgren</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G76" t="n">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="H76" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="78">
@@ -2346,11 +2288,11 @@
     </row>
     <row r="79">
       <c r="B79" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Tennys Sandgren</t>
+          <t>Rafael Nadal</t>
         </is>
       </c>
     </row>

</xml_diff>